<commit_message>
Updated cause id mapping spreadsheet
</commit_message>
<xml_diff>
--- a/docs/Cause id mapping.xlsx
+++ b/docs/Cause id mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf1a48cb1b94a849/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\Rev_project_1\Data-Foundations-Project-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FADFDC0A-53C1-4EB6-A766-45062623D265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD99C677-D7B4-493E-81C2-86B3CC7C1658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9885" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1EBE12F7-0475-4CF7-BF77-7EA37F884EC3}"/>
   </bookViews>
@@ -212,6 +212,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 1</t>
@@ -236,6 +237,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 17</t>
@@ -304,6 +306,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -690,7 +693,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="S17" sqref="S16:S17"/>
+      <selection activeCell="J11" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,5 +1187,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>